<commit_message>
fix bugs for IE9; revise the create page
</commit_message>
<xml_diff>
--- a/grails-app/conf/spreadsheet/CDM_Bulkload_Schematic.xlsx
+++ b/grails-app/conf/spreadsheet/CDM_Bulkload_Schematic.xlsx
@@ -24,14 +24,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="323" uniqueCount="307">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="324" uniqueCount="308">
   <si>
     <t>Consultation Mode</t>
   </si>
   <si>
-    <t>Report Type</t>
-  </si>
-  <si>
     <t>Staff Pennkey</t>
   </si>
   <si>
@@ -41,9 +38,6 @@
     <t>User Goal</t>
   </si>
   <si>
-    <t>User Affiliation</t>
-  </si>
-  <si>
     <t>Interact Times</t>
   </si>
   <si>
@@ -53,9 +47,6 @@
     <t>Event Length (enter in minutes)</t>
   </si>
   <si>
-    <t>User Rank</t>
-  </si>
-  <si>
     <t>Date of Consultation (mm/dd/yyyy)</t>
   </si>
   <si>
@@ -98,9 +89,6 @@
     <t>Course Name</t>
   </si>
   <si>
-    <t xml:space="preserve">Department Affiliation </t>
-  </si>
-  <si>
     <t>Course Number</t>
   </si>
   <si>
@@ -945,6 +933,21 @@
   </si>
   <si>
     <t>Sponsor</t>
+  </si>
+  <si>
+    <t>User Name</t>
+  </si>
+  <si>
+    <t>Rank</t>
+  </si>
+  <si>
+    <t>Library Unit</t>
+  </si>
+  <si>
+    <t>Department</t>
+  </si>
+  <si>
+    <t>School</t>
   </si>
 </sst>
 </file>
@@ -1109,7 +1112,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1149,6 +1152,7 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1450,10 +1454,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:T40"/>
+  <dimension ref="A1:T42"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75"/>
@@ -1468,17 +1472,17 @@
   <sheetData>
     <row r="1" spans="1:20" ht="23.25">
       <c r="A1" s="4" t="s">
-        <v>293</v>
+        <v>289</v>
       </c>
     </row>
     <row r="2" spans="1:20">
       <c r="A2" s="1" t="s">
-        <v>294</v>
+        <v>290</v>
       </c>
     </row>
     <row r="3" spans="1:20">
       <c r="A3" s="13" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
     </row>
     <row r="4" spans="1:20" ht="13.5" customHeight="1">
@@ -1486,51 +1490,51 @@
     </row>
     <row r="6" spans="1:20" ht="15.75">
       <c r="B6" s="19" t="s">
-        <v>1</v>
+        <v>305</v>
       </c>
       <c r="C6" s="20" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="T6" s="1" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
     </row>
     <row r="7" spans="1:20">
       <c r="T7" s="1" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
     <row r="8" spans="1:20" ht="15">
       <c r="B8" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C8" s="22" t="s">
+        <v>291</v>
+      </c>
+      <c r="T8" s="1" t="s">
         <v>10</v>
-      </c>
-      <c r="C8" s="22" t="s">
-        <v>295</v>
-      </c>
-      <c r="T8" s="1" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="9" spans="1:20">
       <c r="B9" s="8"/>
       <c r="T9" s="1" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
     </row>
     <row r="10" spans="1:20" ht="15">
       <c r="B10" s="6" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C10" s="21" t="s">
-        <v>295</v>
+        <v>291</v>
       </c>
       <c r="T10" s="1" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="11" spans="1:20">
       <c r="T11" s="1" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
     </row>
     <row r="12" spans="1:20" ht="15.75">
@@ -1539,153 +1543,167 @@
       </c>
       <c r="C12" s="12"/>
       <c r="T12" s="1" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
     </row>
     <row r="13" spans="1:20">
       <c r="T13" s="1" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
     </row>
     <row r="14" spans="1:20" ht="15.75">
       <c r="B14" s="5" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C14" s="11"/>
       <c r="T14" s="1" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
     </row>
     <row r="15" spans="1:20" ht="18">
       <c r="A15" s="3"/>
       <c r="T15" s="1" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
     </row>
     <row r="16" spans="1:20" ht="15.75">
       <c r="B16" s="5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C16" s="10"/>
       <c r="T16" s="1" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
     </row>
     <row r="17" spans="1:20">
       <c r="T17" s="1" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
     </row>
     <row r="18" spans="1:20" ht="15">
       <c r="B18" s="7" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C18" s="21" t="s">
-        <v>295</v>
+        <v>291</v>
       </c>
     </row>
     <row r="20" spans="1:20" ht="15">
       <c r="B20" s="6" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C20" s="21" t="s">
-        <v>295</v>
-      </c>
+        <v>291</v>
+      </c>
+    </row>
+    <row r="21" spans="1:20" ht="15">
+      <c r="B21" s="6"/>
+      <c r="C21" s="23"/>
     </row>
     <row r="22" spans="1:20" ht="15">
       <c r="B22" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="C22" s="9"/>
-    </row>
-    <row r="24" spans="1:20" ht="18">
-      <c r="A24" s="3"/>
+        <v>303</v>
+      </c>
+      <c r="C22" s="23"/>
+    </row>
+    <row r="24" spans="1:20" ht="15">
       <c r="B24" s="6" t="s">
-        <v>5</v>
+        <v>304</v>
       </c>
       <c r="C24" s="9"/>
     </row>
-    <row r="25" spans="1:20" ht="15">
-      <c r="B25" s="6"/>
-    </row>
-    <row r="26" spans="1:20" ht="15">
+    <row r="26" spans="1:20" ht="18">
+      <c r="A26" s="3"/>
       <c r="B26" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="C26" s="21" t="s">
-        <v>295</v>
-      </c>
+        <v>307</v>
+      </c>
+      <c r="C26" s="9"/>
+    </row>
+    <row r="27" spans="1:20" ht="15">
+      <c r="B27" s="6"/>
     </row>
     <row r="28" spans="1:20" ht="15">
       <c r="B28" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="C28" s="2" t="s">
-        <v>295</v>
-      </c>
-    </row>
-    <row r="29" spans="1:20" ht="15">
-      <c r="B29" s="6"/>
+        <v>4</v>
+      </c>
+      <c r="C28" s="21" t="s">
+        <v>291</v>
+      </c>
     </row>
     <row r="30" spans="1:20" ht="15">
       <c r="B30" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="C30" s="9"/>
+        <v>20</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>291</v>
+      </c>
     </row>
     <row r="31" spans="1:20" ht="15">
       <c r="B31" s="6"/>
     </row>
     <row r="32" spans="1:20" ht="15">
       <c r="B32" s="6" t="s">
+        <v>306</v>
+      </c>
+      <c r="C32" s="9"/>
+    </row>
+    <row r="33" spans="2:4" ht="15">
+      <c r="B33" s="6"/>
+    </row>
+    <row r="34" spans="2:4" ht="15">
+      <c r="B34" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="C34" s="2" t="s">
+        <v>291</v>
+      </c>
+      <c r="D34" s="1"/>
+    </row>
+    <row r="35" spans="2:4" ht="15">
+      <c r="B35" s="6"/>
+      <c r="D35" s="1"/>
+    </row>
+    <row r="36" spans="2:4" ht="15">
+      <c r="B36" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="C36" s="2" t="s">
+        <v>291</v>
+      </c>
+      <c r="D36" s="1"/>
+    </row>
+    <row r="37" spans="2:4" ht="15">
+      <c r="B37" s="6"/>
+      <c r="D37" s="1"/>
+    </row>
+    <row r="38" spans="2:4" ht="15">
+      <c r="B38" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="C38" s="9"/>
+      <c r="D38" s="1"/>
+    </row>
+    <row r="39" spans="2:4" ht="15">
+      <c r="B39" s="6"/>
+      <c r="D39" s="1"/>
+    </row>
+    <row r="40" spans="2:4" ht="15">
+      <c r="B40" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="C40" s="2" t="s">
+        <v>291</v>
+      </c>
+      <c r="D40" s="1"/>
+    </row>
+    <row r="42" spans="2:4" ht="15">
+      <c r="B42" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="C32" s="2" t="s">
-        <v>295</v>
-      </c>
-      <c r="D32" s="1"/>
-    </row>
-    <row r="33" spans="2:3" s="1" customFormat="1" ht="15">
-      <c r="B33" s="6"/>
-      <c r="C33" s="2"/>
-    </row>
-    <row r="34" spans="2:3" s="1" customFormat="1" ht="15">
-      <c r="B34" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="C34" s="2" t="s">
-        <v>295</v>
-      </c>
-    </row>
-    <row r="35" spans="2:3" s="1" customFormat="1" ht="15">
-      <c r="B35" s="6"/>
-      <c r="C35" s="2"/>
-    </row>
-    <row r="36" spans="2:3" s="1" customFormat="1" ht="15">
-      <c r="B36" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="C36" s="9"/>
-    </row>
-    <row r="37" spans="2:3" s="1" customFormat="1" ht="15">
-      <c r="B37" s="6"/>
-      <c r="C37" s="2"/>
-    </row>
-    <row r="38" spans="2:3" s="1" customFormat="1" ht="15">
-      <c r="B38" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="C38" s="2" t="s">
-        <v>295</v>
-      </c>
-    </row>
-    <row r="40" spans="2:3" s="1" customFormat="1" ht="15">
-      <c r="B40" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="C40" s="2" t="s">
-        <v>295</v>
-      </c>
+      <c r="C42" s="2" t="s">
+        <v>291</v>
+      </c>
+      <c r="D42" s="1"/>
     </row>
   </sheetData>
   <dataValidations count="7">
@@ -1701,13 +1719,13 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="User Goal" prompt="Select One" sqref="C16">
       <formula1>GOAL</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="User" prompt="Select one" sqref="C22">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="User" prompt="Select one" sqref="C24">
       <formula1>USER</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="User Affiliation" prompt="Select One" sqref="C24">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="User Affiliation" prompt="Select One" sqref="C26">
       <formula1>"SAS, SEAS, Wharton, GSE, Vet, Nursing, Med, Dental, SP2, Design, UPHS, CHOP, Annenberg, Law, Penn Other (Please Indicate), Outside Penn (Please Indicate)"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C30">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C32">
       <formula1>DeptList</formula1>
     </dataValidation>
   </dataValidations>
@@ -1720,7 +1738,7 @@
           <x14:formula1>
             <xm:f>CDMService!$F$3:$F$16</xm:f>
           </x14:formula1>
-          <xm:sqref>C36</xm:sqref>
+          <xm:sqref>C38</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -1744,1107 +1762,1107 @@
     <row r="2" spans="2:2" ht="15.75" thickBot="1"/>
     <row r="3" spans="2:2" ht="16.5" thickBot="1">
       <c r="B3" s="14" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
     </row>
     <row r="4" spans="2:2" ht="16.5" thickBot="1">
       <c r="B4" s="15" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
     </row>
     <row r="5" spans="2:2" ht="16.5" thickBot="1">
       <c r="B5" s="15" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
     </row>
     <row r="6" spans="2:2" ht="16.5" thickBot="1">
       <c r="B6" s="15" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
     </row>
     <row r="7" spans="2:2" ht="16.5" thickBot="1">
       <c r="B7" s="15" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
     </row>
     <row r="8" spans="2:2" ht="16.5" thickBot="1">
       <c r="B8" s="15" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
     </row>
     <row r="9" spans="2:2" ht="16.5" thickBot="1">
       <c r="B9" s="15" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
     </row>
     <row r="10" spans="2:2" ht="16.5" thickBot="1">
       <c r="B10" s="15" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
     </row>
     <row r="11" spans="2:2" ht="16.5" thickBot="1">
       <c r="B11" s="15" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
     </row>
     <row r="12" spans="2:2" ht="16.5" thickBot="1">
       <c r="B12" s="15" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
     </row>
     <row r="13" spans="2:2" ht="16.5" thickBot="1">
       <c r="B13" s="15" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
     </row>
     <row r="14" spans="2:2" ht="16.5" thickBot="1">
       <c r="B14" s="15" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
     </row>
     <row r="15" spans="2:2" ht="16.5" thickBot="1">
       <c r="B15" s="15" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
     </row>
     <row r="16" spans="2:2" ht="16.5" thickBot="1">
       <c r="B16" s="15" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
     </row>
     <row r="17" spans="2:2" ht="16.5" thickBot="1">
       <c r="B17" s="15" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
     </row>
     <row r="18" spans="2:2" ht="16.5" thickBot="1">
       <c r="B18" s="15" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
     </row>
     <row r="19" spans="2:2" ht="16.5" thickBot="1">
       <c r="B19" s="15" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
     </row>
     <row r="20" spans="2:2" ht="16.5" thickBot="1">
       <c r="B20" s="15" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
     </row>
     <row r="21" spans="2:2" ht="16.5" thickBot="1">
       <c r="B21" s="15" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
     </row>
     <row r="22" spans="2:2" ht="16.5" thickBot="1">
       <c r="B22" s="15" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
     </row>
     <row r="23" spans="2:2" ht="16.5" thickBot="1">
       <c r="B23" s="15" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
     </row>
     <row r="24" spans="2:2" ht="16.5" thickBot="1">
       <c r="B24" s="15" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
     </row>
     <row r="25" spans="2:2" ht="16.5" thickBot="1">
       <c r="B25" s="15" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
     </row>
     <row r="26" spans="2:2" ht="16.5" thickBot="1">
       <c r="B26" s="15" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
     </row>
     <row r="27" spans="2:2" ht="16.5" thickBot="1">
       <c r="B27" s="15" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
     </row>
     <row r="28" spans="2:2" ht="16.5" thickBot="1">
       <c r="B28" s="15" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
     </row>
     <row r="29" spans="2:2" ht="16.5" thickBot="1">
       <c r="B29" s="15" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
     </row>
     <row r="30" spans="2:2" ht="16.5" thickBot="1">
       <c r="B30" s="15" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
     </row>
     <row r="31" spans="2:2" ht="16.5" thickBot="1">
       <c r="B31" s="15" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
     </row>
     <row r="32" spans="2:2" ht="16.5" thickBot="1">
       <c r="B32" s="15" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
     </row>
     <row r="33" spans="2:2" ht="16.5" thickBot="1">
       <c r="B33" s="15" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
     </row>
     <row r="34" spans="2:2" ht="16.5" thickBot="1">
       <c r="B34" s="15" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
     </row>
     <row r="35" spans="2:2" ht="16.5" thickBot="1">
       <c r="B35" s="15" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
     </row>
     <row r="36" spans="2:2" ht="16.5" thickBot="1">
       <c r="B36" s="15" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
     </row>
     <row r="37" spans="2:2" ht="16.5" thickBot="1">
       <c r="B37" s="15" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
     </row>
     <row r="38" spans="2:2" ht="16.5" thickBot="1">
       <c r="B38" s="15" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
     </row>
     <row r="39" spans="2:2" ht="16.5" thickBot="1">
       <c r="B39" s="15" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
     </row>
     <row r="40" spans="2:2" ht="16.5" thickBot="1">
       <c r="B40" s="15" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
     </row>
     <row r="41" spans="2:2" ht="16.5" thickBot="1">
       <c r="B41" s="15" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
     </row>
     <row r="42" spans="2:2" ht="16.5" thickBot="1">
       <c r="B42" s="15" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
     </row>
     <row r="43" spans="2:2" ht="16.5" thickBot="1">
       <c r="B43" s="15" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
     </row>
     <row r="44" spans="2:2" ht="16.5" thickBot="1">
       <c r="B44" s="15" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
     </row>
     <row r="45" spans="2:2" ht="16.5" thickBot="1">
       <c r="B45" s="15" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
     </row>
     <row r="46" spans="2:2" ht="16.5" thickBot="1">
       <c r="B46" s="15" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
     </row>
     <row r="47" spans="2:2" ht="16.5" thickBot="1">
       <c r="B47" s="15" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
     </row>
     <row r="48" spans="2:2" ht="16.5" thickBot="1">
       <c r="B48" s="15" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
     </row>
     <row r="49" spans="2:2" ht="16.5" thickBot="1">
       <c r="B49" s="15" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
     </row>
     <row r="50" spans="2:2" ht="16.5" thickBot="1">
       <c r="B50" s="15" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
     </row>
     <row r="51" spans="2:2" ht="16.5" thickBot="1">
       <c r="B51" s="15" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
     </row>
     <row r="52" spans="2:2" ht="16.5" thickBot="1">
       <c r="B52" s="15" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
     </row>
     <row r="53" spans="2:2" ht="16.5" thickBot="1">
       <c r="B53" s="15" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
     </row>
     <row r="54" spans="2:2" ht="16.5" thickBot="1">
       <c r="B54" s="15" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
     </row>
     <row r="55" spans="2:2" ht="16.5" thickBot="1">
       <c r="B55" s="15" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
     </row>
     <row r="56" spans="2:2" ht="16.5" thickBot="1">
       <c r="B56" s="15" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
     </row>
     <row r="57" spans="2:2" ht="16.5" thickBot="1">
       <c r="B57" s="15" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
     </row>
     <row r="58" spans="2:2" ht="16.5" thickBot="1">
       <c r="B58" s="15" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
     </row>
     <row r="59" spans="2:2" ht="16.5" thickBot="1">
       <c r="B59" s="15" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
     </row>
     <row r="60" spans="2:2" ht="16.5" thickBot="1">
       <c r="B60" s="15" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
     </row>
     <row r="61" spans="2:2" ht="16.5" thickBot="1">
       <c r="B61" s="15" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
     </row>
     <row r="62" spans="2:2" ht="16.5" thickBot="1">
       <c r="B62" s="15" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
     </row>
     <row r="63" spans="2:2" ht="16.5" thickBot="1">
       <c r="B63" s="15" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
     </row>
     <row r="64" spans="2:2" ht="16.5" thickBot="1">
       <c r="B64" s="15" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
     </row>
     <row r="65" spans="2:2" ht="16.5" thickBot="1">
       <c r="B65" s="15" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
     </row>
     <row r="66" spans="2:2" ht="16.5" thickBot="1">
       <c r="B66" s="15" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
     </row>
     <row r="67" spans="2:2" ht="16.5" thickBot="1">
       <c r="B67" s="15" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
     </row>
     <row r="68" spans="2:2" ht="16.5" thickBot="1">
       <c r="B68" s="15" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
     </row>
     <row r="69" spans="2:2" ht="16.5" thickBot="1">
       <c r="B69" s="15" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
     </row>
     <row r="70" spans="2:2" ht="16.5" thickBot="1">
       <c r="B70" s="15" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
     </row>
     <row r="71" spans="2:2" ht="16.5" thickBot="1">
       <c r="B71" s="15" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
     </row>
     <row r="72" spans="2:2" ht="16.5" thickBot="1">
       <c r="B72" s="15" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
     </row>
     <row r="73" spans="2:2" ht="16.5" thickBot="1">
       <c r="B73" s="15" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
     </row>
     <row r="74" spans="2:2" ht="16.5" thickBot="1">
       <c r="B74" s="15" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
     </row>
     <row r="75" spans="2:2" ht="16.5" thickBot="1">
       <c r="B75" s="15" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
     </row>
     <row r="76" spans="2:2" ht="16.5" thickBot="1">
       <c r="B76" s="15" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
     </row>
     <row r="77" spans="2:2" ht="16.5" thickBot="1">
       <c r="B77" s="15" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
     </row>
     <row r="78" spans="2:2" ht="16.5" thickBot="1">
       <c r="B78" s="15" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
     </row>
     <row r="79" spans="2:2" ht="16.5" thickBot="1">
       <c r="B79" s="15" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
     </row>
     <row r="80" spans="2:2" ht="16.5" thickBot="1">
       <c r="B80" s="15" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
     </row>
     <row r="81" spans="2:2" ht="16.5" thickBot="1">
       <c r="B81" s="15" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
     </row>
     <row r="82" spans="2:2" ht="16.5" thickBot="1">
       <c r="B82" s="15" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
     </row>
     <row r="83" spans="2:2" ht="16.5" thickBot="1">
       <c r="B83" s="15" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
     </row>
     <row r="84" spans="2:2" ht="16.5" thickBot="1">
       <c r="B84" s="15" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
     </row>
     <row r="85" spans="2:2" ht="16.5" thickBot="1">
       <c r="B85" s="15" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
     </row>
     <row r="86" spans="2:2" ht="16.5" thickBot="1">
       <c r="B86" s="15" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
     </row>
     <row r="87" spans="2:2" ht="16.5" thickBot="1">
       <c r="B87" s="15" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
     </row>
     <row r="88" spans="2:2" ht="16.5" thickBot="1">
       <c r="B88" s="15" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
     </row>
     <row r="89" spans="2:2" ht="16.5" thickBot="1">
       <c r="B89" s="15" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
     </row>
     <row r="90" spans="2:2" ht="16.5" thickBot="1">
       <c r="B90" s="15" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
     </row>
     <row r="91" spans="2:2" ht="16.5" thickBot="1">
       <c r="B91" s="15" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
     </row>
     <row r="92" spans="2:2" ht="16.5" thickBot="1">
       <c r="B92" s="15" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
     </row>
     <row r="93" spans="2:2" ht="16.5" thickBot="1">
       <c r="B93" s="15" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
     </row>
     <row r="94" spans="2:2" ht="16.5" thickBot="1">
       <c r="B94" s="15" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
     </row>
     <row r="95" spans="2:2" ht="16.5" thickBot="1">
       <c r="B95" s="15" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
     </row>
     <row r="96" spans="2:2" ht="16.5" thickBot="1">
       <c r="B96" s="15" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
     </row>
     <row r="97" spans="2:2" ht="16.5" thickBot="1">
       <c r="B97" s="15" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
     </row>
     <row r="98" spans="2:2" ht="16.5" thickBot="1">
       <c r="B98" s="15" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
     </row>
     <row r="99" spans="2:2" ht="16.5" thickBot="1">
       <c r="B99" s="15" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
     </row>
     <row r="100" spans="2:2" ht="16.5" thickBot="1">
       <c r="B100" s="15" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
     </row>
     <row r="101" spans="2:2" ht="16.5" thickBot="1">
       <c r="B101" s="15" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
     </row>
     <row r="102" spans="2:2" ht="16.5" thickBot="1">
       <c r="B102" s="15" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
     </row>
     <row r="103" spans="2:2" ht="16.5" thickBot="1">
       <c r="B103" s="15" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
     </row>
     <row r="104" spans="2:2" ht="16.5" thickBot="1">
       <c r="B104" s="15" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
     </row>
     <row r="105" spans="2:2" ht="16.5" thickBot="1">
       <c r="B105" s="15" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
     </row>
     <row r="106" spans="2:2" ht="16.5" thickBot="1">
       <c r="B106" s="15" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
     </row>
     <row r="107" spans="2:2" ht="16.5" thickBot="1">
       <c r="B107" s="15" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
     </row>
     <row r="108" spans="2:2" ht="16.5" thickBot="1">
       <c r="B108" s="15" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
     </row>
     <row r="109" spans="2:2" ht="16.5" thickBot="1">
       <c r="B109" s="15" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
     </row>
     <row r="110" spans="2:2" ht="16.5" thickBot="1">
       <c r="B110" s="15" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
     </row>
     <row r="111" spans="2:2" ht="16.5" thickBot="1">
       <c r="B111" s="15" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
     </row>
     <row r="112" spans="2:2" ht="16.5" thickBot="1">
       <c r="B112" s="15" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
     </row>
     <row r="113" spans="2:2" ht="16.5" thickBot="1">
       <c r="B113" s="15" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
     </row>
     <row r="114" spans="2:2" ht="16.5" thickBot="1">
       <c r="B114" s="15" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
     </row>
     <row r="115" spans="2:2" ht="16.5" thickBot="1">
       <c r="B115" s="15" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
     </row>
     <row r="116" spans="2:2" ht="16.5" thickBot="1">
       <c r="B116" s="15" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
     </row>
     <row r="117" spans="2:2" ht="16.5" thickBot="1">
       <c r="B117" s="15" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
     </row>
     <row r="118" spans="2:2" ht="16.5" thickBot="1">
       <c r="B118" s="15" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
     </row>
     <row r="119" spans="2:2" ht="16.5" thickBot="1">
       <c r="B119" s="15" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
     </row>
     <row r="120" spans="2:2" ht="16.5" thickBot="1">
       <c r="B120" s="15" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
     </row>
     <row r="121" spans="2:2" ht="16.5" thickBot="1">
       <c r="B121" s="15" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
     </row>
     <row r="122" spans="2:2" ht="16.5" thickBot="1">
       <c r="B122" s="15" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
     </row>
     <row r="123" spans="2:2" ht="16.5" thickBot="1">
       <c r="B123" s="15" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
     </row>
     <row r="124" spans="2:2" ht="16.5" thickBot="1">
       <c r="B124" s="15" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
     </row>
     <row r="125" spans="2:2" ht="16.5" thickBot="1">
       <c r="B125" s="15" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
     </row>
     <row r="126" spans="2:2" ht="16.5" thickBot="1">
       <c r="B126" s="15" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
     </row>
     <row r="127" spans="2:2" ht="16.5" thickBot="1">
       <c r="B127" s="15" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
     </row>
     <row r="128" spans="2:2" ht="16.5" thickBot="1">
       <c r="B128" s="15" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
     </row>
     <row r="129" spans="2:2" ht="16.5" thickBot="1">
       <c r="B129" s="15" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
     </row>
     <row r="130" spans="2:2" ht="16.5" thickBot="1">
       <c r="B130" s="15" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
     </row>
     <row r="131" spans="2:2" ht="16.5" thickBot="1">
       <c r="B131" s="15" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
     </row>
     <row r="132" spans="2:2" ht="16.5" thickBot="1">
       <c r="B132" s="15" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
     </row>
     <row r="133" spans="2:2" ht="16.5" thickBot="1">
       <c r="B133" s="15" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
     </row>
     <row r="134" spans="2:2" ht="16.5" thickBot="1">
       <c r="B134" s="15" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
     </row>
     <row r="135" spans="2:2" ht="16.5" thickBot="1">
       <c r="B135" s="15" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
     </row>
     <row r="136" spans="2:2" ht="16.5" thickBot="1">
       <c r="B136" s="15" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
     </row>
     <row r="137" spans="2:2" ht="16.5" thickBot="1">
       <c r="B137" s="15" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
     </row>
     <row r="138" spans="2:2" ht="16.5" thickBot="1">
       <c r="B138" s="15" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
     </row>
     <row r="139" spans="2:2" ht="16.5" thickBot="1">
       <c r="B139" s="15" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
     </row>
     <row r="140" spans="2:2" ht="16.5" thickBot="1">
       <c r="B140" s="15" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
     </row>
     <row r="141" spans="2:2" ht="16.5" thickBot="1">
       <c r="B141" s="15" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
     </row>
     <row r="142" spans="2:2" ht="16.5" thickBot="1">
       <c r="B142" s="15" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
     </row>
     <row r="143" spans="2:2" ht="16.5" thickBot="1">
       <c r="B143" s="15" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
     </row>
     <row r="144" spans="2:2" ht="16.5" thickBot="1">
       <c r="B144" s="15" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
     </row>
     <row r="145" spans="2:2" ht="16.5" thickBot="1">
       <c r="B145" s="15" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
     </row>
     <row r="146" spans="2:2" ht="16.5" thickBot="1">
       <c r="B146" s="15" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
     </row>
     <row r="147" spans="2:2" ht="16.5" thickBot="1">
       <c r="B147" s="15" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
     </row>
     <row r="148" spans="2:2" ht="16.5" thickBot="1">
       <c r="B148" s="15" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
     </row>
     <row r="149" spans="2:2" ht="16.5" thickBot="1">
       <c r="B149" s="15" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
     </row>
     <row r="150" spans="2:2" ht="16.5" thickBot="1">
       <c r="B150" s="15" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
     </row>
     <row r="151" spans="2:2" ht="16.5" thickBot="1">
       <c r="B151" s="15" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
     </row>
     <row r="152" spans="2:2" ht="16.5" thickBot="1">
       <c r="B152" s="15" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
     </row>
     <row r="153" spans="2:2" ht="16.5" thickBot="1">
       <c r="B153" s="15" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
     </row>
     <row r="154" spans="2:2" ht="16.5" thickBot="1">
       <c r="B154" s="15" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
     </row>
     <row r="155" spans="2:2" ht="16.5" thickBot="1">
       <c r="B155" s="15" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
     </row>
     <row r="156" spans="2:2" ht="16.5" thickBot="1">
       <c r="B156" s="15" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
     </row>
     <row r="157" spans="2:2" ht="16.5" thickBot="1">
       <c r="B157" s="15" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
     </row>
     <row r="158" spans="2:2" ht="16.5" thickBot="1">
       <c r="B158" s="15" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
     </row>
     <row r="159" spans="2:2" ht="16.5" thickBot="1">
       <c r="B159" s="15" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
     </row>
     <row r="160" spans="2:2" ht="16.5" thickBot="1">
       <c r="B160" s="15" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
     </row>
     <row r="161" spans="2:2" ht="16.5" thickBot="1">
       <c r="B161" s="15" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
     </row>
     <row r="162" spans="2:2" ht="16.5" thickBot="1">
       <c r="B162" s="15" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
     </row>
     <row r="163" spans="2:2" ht="16.5" thickBot="1">
       <c r="B163" s="15" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
     </row>
     <row r="164" spans="2:2" ht="16.5" thickBot="1">
       <c r="B164" s="15" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
     </row>
     <row r="165" spans="2:2" ht="16.5" thickBot="1">
       <c r="B165" s="15" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
     </row>
     <row r="166" spans="2:2" ht="16.5" thickBot="1">
       <c r="B166" s="15" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
     </row>
     <row r="167" spans="2:2" ht="16.5" thickBot="1">
       <c r="B167" s="15" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
     </row>
     <row r="168" spans="2:2" ht="16.5" thickBot="1">
       <c r="B168" s="15" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
     </row>
     <row r="169" spans="2:2" ht="16.5" thickBot="1">
       <c r="B169" s="15" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
     </row>
     <row r="170" spans="2:2" ht="16.5" thickBot="1">
       <c r="B170" s="15" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
     </row>
     <row r="171" spans="2:2" ht="16.5" thickBot="1">
       <c r="B171" s="15" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
     </row>
     <row r="172" spans="2:2" ht="16.5" thickBot="1">
       <c r="B172" s="15" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
     </row>
     <row r="173" spans="2:2" ht="16.5" thickBot="1">
       <c r="B173" s="15" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
     </row>
     <row r="174" spans="2:2" ht="16.5" thickBot="1">
       <c r="B174" s="15" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
     </row>
     <row r="175" spans="2:2" ht="16.5" thickBot="1">
       <c r="B175" s="15" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
     </row>
     <row r="176" spans="2:2" ht="16.5" thickBot="1">
       <c r="B176" s="15" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
     </row>
     <row r="177" spans="2:2" ht="16.5" thickBot="1">
       <c r="B177" s="15" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
     </row>
     <row r="178" spans="2:2" ht="16.5" thickBot="1">
       <c r="B178" s="15" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
     </row>
     <row r="179" spans="2:2" ht="16.5" thickBot="1">
       <c r="B179" s="15" t="s">
-        <v>207</v>
+        <v>203</v>
       </c>
     </row>
     <row r="180" spans="2:2" ht="16.5" thickBot="1">
       <c r="B180" s="15" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
     </row>
     <row r="181" spans="2:2" ht="16.5" thickBot="1">
       <c r="B181" s="15" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
     </row>
     <row r="182" spans="2:2" ht="16.5" thickBot="1">
       <c r="B182" s="15" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
     </row>
     <row r="183" spans="2:2" ht="16.5" thickBot="1">
       <c r="B183" s="15" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
     </row>
     <row r="184" spans="2:2" ht="16.5" thickBot="1">
       <c r="B184" s="15" t="s">
-        <v>212</v>
+        <v>208</v>
       </c>
     </row>
     <row r="185" spans="2:2" ht="16.5" thickBot="1">
       <c r="B185" s="15" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
     </row>
     <row r="186" spans="2:2" ht="16.5" thickBot="1">
       <c r="B186" s="15" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
     </row>
     <row r="187" spans="2:2" ht="16.5" thickBot="1">
       <c r="B187" s="15" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
     </row>
     <row r="188" spans="2:2" ht="16.5" thickBot="1">
       <c r="B188" s="15" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
     </row>
     <row r="189" spans="2:2" ht="16.5" thickBot="1">
       <c r="B189" s="15" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
     </row>
     <row r="190" spans="2:2" ht="16.5" thickBot="1">
       <c r="B190" s="15" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
     </row>
     <row r="191" spans="2:2" ht="16.5" thickBot="1">
       <c r="B191" s="15" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
     </row>
     <row r="192" spans="2:2" ht="16.5" thickBot="1">
       <c r="B192" s="15" t="s">
-        <v>219</v>
+        <v>215</v>
       </c>
     </row>
     <row r="193" spans="2:2" ht="16.5" thickBot="1">
       <c r="B193" s="15" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
     </row>
     <row r="194" spans="2:2" ht="16.5" thickBot="1">
       <c r="B194" s="15" t="s">
-        <v>221</v>
+        <v>217</v>
       </c>
     </row>
     <row r="195" spans="2:2" ht="16.5" thickBot="1">
       <c r="B195" s="15" t="s">
-        <v>222</v>
+        <v>218</v>
       </c>
     </row>
     <row r="196" spans="2:2" ht="16.5" thickBot="1">
       <c r="B196" s="15" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
     </row>
     <row r="197" spans="2:2" ht="16.5" thickBot="1">
       <c r="B197" s="15" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
     </row>
     <row r="198" spans="2:2" ht="16.5" thickBot="1">
       <c r="B198" s="15" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
     </row>
     <row r="199" spans="2:2" ht="16.5" thickBot="1">
       <c r="B199" s="15" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
     </row>
     <row r="200" spans="2:2" ht="16.5" thickBot="1">
       <c r="B200" s="15" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
     </row>
     <row r="201" spans="2:2" ht="16.5" thickBot="1">
       <c r="B201" s="15" t="s">
-        <v>228</v>
+        <v>224</v>
       </c>
     </row>
     <row r="202" spans="2:2" ht="16.5" thickBot="1">
       <c r="B202" s="15" t="s">
-        <v>229</v>
+        <v>225</v>
       </c>
     </row>
     <row r="203" spans="2:2" ht="16.5" thickBot="1">
       <c r="B203" s="15" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
     </row>
     <row r="204" spans="2:2" ht="16.5" thickBot="1">
       <c r="B204" s="15" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
     </row>
     <row r="205" spans="2:2" ht="16.5" thickBot="1">
       <c r="B205" s="15" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
     </row>
     <row r="206" spans="2:2" ht="16.5" thickBot="1">
       <c r="B206" s="15" t="s">
-        <v>233</v>
+        <v>229</v>
       </c>
     </row>
     <row r="207" spans="2:2" ht="16.5" thickBot="1">
       <c r="B207" s="15" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
     </row>
     <row r="208" spans="2:2" ht="16.5" thickBot="1">
       <c r="B208" s="15" t="s">
-        <v>235</v>
+        <v>231</v>
       </c>
     </row>
     <row r="209" spans="2:2" ht="16.5" thickBot="1">
       <c r="B209" s="15" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
     </row>
     <row r="210" spans="2:2" ht="16.5" thickBot="1">
       <c r="B210" s="15" t="s">
-        <v>237</v>
+        <v>233</v>
       </c>
     </row>
     <row r="211" spans="2:2" ht="16.5" thickBot="1">
       <c r="B211" s="15" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
     </row>
     <row r="212" spans="2:2" ht="16.5" thickBot="1">
       <c r="B212" s="15" t="s">
-        <v>238</v>
+        <v>234</v>
       </c>
     </row>
     <row r="213" spans="2:2" ht="16.5" thickBot="1">
       <c r="B213" s="15" t="s">
-        <v>239</v>
+        <v>235</v>
       </c>
     </row>
     <row r="214" spans="2:2" ht="16.5" thickBot="1">
       <c r="B214" s="15" t="s">
-        <v>240</v>
+        <v>236</v>
       </c>
     </row>
     <row r="215" spans="2:2" ht="16.5" thickBot="1">
       <c r="B215" s="15" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
     </row>
     <row r="216" spans="2:2" ht="16.5" thickBot="1">
       <c r="B216" s="15" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
     </row>
     <row r="217" spans="2:2" ht="16.5" thickBot="1">
       <c r="B217" s="15" t="s">
-        <v>243</v>
+        <v>239</v>
       </c>
     </row>
     <row r="218" spans="2:2" ht="16.5" thickBot="1">
       <c r="B218" s="15" t="s">
-        <v>244</v>
+        <v>240</v>
       </c>
     </row>
     <row r="219" spans="2:2" ht="16.5" thickBot="1">
       <c r="B219" s="15" t="s">
-        <v>245</v>
+        <v>241</v>
       </c>
     </row>
     <row r="220" spans="2:2" ht="16.5" thickBot="1">
       <c r="B220" s="15" t="s">
-        <v>246</v>
+        <v>242</v>
       </c>
     </row>
     <row r="221" spans="2:2" ht="16.5" thickBot="1">
       <c r="B221" s="15" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
     </row>
     <row r="222" spans="2:2" ht="16.5" thickBot="1">
       <c r="B222" s="15" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
     </row>
     <row r="223" spans="2:2" ht="16.5" thickBot="1">
       <c r="B223" s="15" t="s">
-        <v>249</v>
+        <v>245</v>
       </c>
     </row>
   </sheetData>
@@ -2871,220 +2889,220 @@
   <sheetData>
     <row r="2" spans="2:6">
       <c r="B2" s="16" t="s">
-        <v>271</v>
+        <v>267</v>
       </c>
       <c r="C2" s="18" t="s">
-        <v>272</v>
+        <v>268</v>
       </c>
       <c r="D2" s="18" t="s">
-        <v>274</v>
+        <v>270</v>
       </c>
       <c r="E2" s="18" t="s">
-        <v>273</v>
+        <v>269</v>
       </c>
       <c r="F2" s="18" t="s">
-        <v>306</v>
+        <v>302</v>
       </c>
     </row>
     <row r="3" spans="2:6">
       <c r="B3" t="s">
-        <v>250</v>
+        <v>246</v>
       </c>
       <c r="C3" t="s">
-        <v>275</v>
+        <v>271</v>
       </c>
       <c r="D3" t="s">
-        <v>276</v>
+        <v>272</v>
       </c>
       <c r="E3" s="17" t="s">
-        <v>289</v>
+        <v>285</v>
       </c>
       <c r="F3" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
     </row>
     <row r="4" spans="2:6">
       <c r="B4" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
       <c r="C4" t="s">
-        <v>277</v>
+        <v>273</v>
       </c>
       <c r="D4" t="s">
-        <v>278</v>
+        <v>274</v>
       </c>
       <c r="E4" s="17" t="s">
-        <v>290</v>
+        <v>286</v>
       </c>
       <c r="F4" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
     </row>
     <row r="5" spans="2:6">
       <c r="B5" t="s">
-        <v>252</v>
+        <v>248</v>
       </c>
       <c r="C5" t="s">
-        <v>279</v>
+        <v>275</v>
       </c>
       <c r="D5" t="s">
-        <v>280</v>
+        <v>276</v>
       </c>
       <c r="E5" s="17" t="s">
-        <v>291</v>
+        <v>287</v>
       </c>
       <c r="F5" t="s">
-        <v>296</v>
+        <v>292</v>
       </c>
     </row>
     <row r="6" spans="2:6">
       <c r="B6" t="s">
-        <v>253</v>
+        <v>249</v>
       </c>
       <c r="C6" t="s">
-        <v>281</v>
+        <v>277</v>
       </c>
       <c r="D6" t="s">
-        <v>282</v>
+        <v>278</v>
       </c>
       <c r="E6" s="17" t="s">
-        <v>292</v>
+        <v>288</v>
       </c>
       <c r="F6" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
     </row>
     <row r="7" spans="2:6">
       <c r="B7" t="s">
-        <v>254</v>
+        <v>250</v>
       </c>
       <c r="C7" t="s">
-        <v>283</v>
+        <v>279</v>
       </c>
       <c r="D7" t="s">
-        <v>284</v>
+        <v>280</v>
       </c>
       <c r="F7" t="s">
-        <v>297</v>
+        <v>293</v>
       </c>
     </row>
     <row r="8" spans="2:6">
       <c r="B8" t="s">
-        <v>255</v>
+        <v>251</v>
       </c>
       <c r="C8" t="s">
-        <v>285</v>
+        <v>281</v>
       </c>
       <c r="D8" t="s">
-        <v>286</v>
+        <v>282</v>
       </c>
       <c r="F8" t="s">
-        <v>298</v>
+        <v>294</v>
       </c>
     </row>
     <row r="9" spans="2:6">
       <c r="B9" t="s">
-        <v>256</v>
+        <v>252</v>
       </c>
       <c r="D9" t="s">
-        <v>287</v>
+        <v>283</v>
       </c>
       <c r="F9" t="s">
-        <v>299</v>
+        <v>295</v>
       </c>
     </row>
     <row r="10" spans="2:6">
       <c r="B10" t="s">
-        <v>257</v>
+        <v>253</v>
       </c>
       <c r="D10" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
       <c r="F10" t="s">
-        <v>300</v>
+        <v>296</v>
       </c>
     </row>
     <row r="11" spans="2:6">
       <c r="B11" t="s">
-        <v>258</v>
+        <v>254</v>
       </c>
       <c r="F11" t="s">
-        <v>301</v>
+        <v>297</v>
       </c>
     </row>
     <row r="12" spans="2:6">
       <c r="B12" t="s">
-        <v>259</v>
+        <v>255</v>
       </c>
       <c r="F12" t="s">
-        <v>302</v>
+        <v>298</v>
       </c>
     </row>
     <row r="13" spans="2:6">
       <c r="B13" t="s">
-        <v>260</v>
+        <v>256</v>
       </c>
       <c r="F13" t="s">
-        <v>303</v>
+        <v>299</v>
       </c>
     </row>
     <row r="14" spans="2:6">
       <c r="B14" t="s">
-        <v>261</v>
+        <v>257</v>
       </c>
       <c r="F14" t="s">
-        <v>304</v>
+        <v>300</v>
       </c>
     </row>
     <row r="15" spans="2:6">
       <c r="B15" t="s">
-        <v>262</v>
+        <v>258</v>
       </c>
       <c r="F15" t="s">
-        <v>305</v>
+        <v>301</v>
       </c>
     </row>
     <row r="16" spans="2:6">
       <c r="B16" t="s">
-        <v>263</v>
+        <v>259</v>
       </c>
       <c r="F16" t="s">
-        <v>292</v>
+        <v>288</v>
       </c>
     </row>
     <row r="17" spans="2:2">
       <c r="B17" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
     </row>
     <row r="18" spans="2:2">
       <c r="B18" t="s">
-        <v>265</v>
+        <v>261</v>
       </c>
     </row>
     <row r="19" spans="2:2">
       <c r="B19" t="s">
-        <v>266</v>
+        <v>262</v>
       </c>
     </row>
     <row r="20" spans="2:2">
       <c r="B20" t="s">
-        <v>267</v>
+        <v>263</v>
       </c>
     </row>
     <row r="21" spans="2:2">
       <c r="B21" t="s">
-        <v>268</v>
+        <v>264</v>
       </c>
     </row>
     <row r="22" spans="2:2">
       <c r="B22" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
     </row>
     <row r="23" spans="2:2">
       <c r="B23" t="s">
-        <v>270</v>
+        <v>266</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
changes according to Joe's feedback
</commit_message>
<xml_diff>
--- a/grails-app/conf/spreadsheet/CDM_Bulkload_Schematic.xlsx
+++ b/grails-app/conf/spreadsheet/CDM_Bulkload_Schematic.xlsx
@@ -38,9 +38,6 @@
     <t>User Goal</t>
   </si>
   <si>
-    <t>Interact Times</t>
-  </si>
-  <si>
     <t>Prep Time (enter in minutes)</t>
   </si>
   <si>
@@ -948,6 +945,9 @@
   </si>
   <si>
     <t>School</t>
+  </si>
+  <si>
+    <t>Interact Occurrences</t>
   </si>
 </sst>
 </file>
@@ -1456,8 +1456,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="B26" sqref="B26"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75"/>
@@ -1472,17 +1472,17 @@
   <sheetData>
     <row r="1" spans="1:20" ht="23.25">
       <c r="A1" s="4" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
     </row>
     <row r="2" spans="1:20">
       <c r="A2" s="1" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
     </row>
     <row r="3" spans="1:20">
       <c r="A3" s="13" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="4" spans="1:20" ht="13.5" customHeight="1">
@@ -1490,35 +1490,35 @@
     </row>
     <row r="6" spans="1:20" ht="15.75">
       <c r="B6" s="19" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="C6" s="20" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="T6" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="7" spans="1:20">
       <c r="T7" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="8" spans="1:20" ht="15">
       <c r="B8" s="6" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C8" s="22" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="T8" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="9" spans="1:20">
       <c r="B9" s="8"/>
       <c r="T9" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="10" spans="1:20" ht="15">
@@ -1526,15 +1526,15 @@
         <v>1</v>
       </c>
       <c r="C10" s="21" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="T10" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="11" spans="1:20">
       <c r="T11" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="12" spans="1:20" ht="15.75">
@@ -1543,12 +1543,12 @@
       </c>
       <c r="C12" s="12"/>
       <c r="T12" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="13" spans="1:20">
       <c r="T13" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="14" spans="1:20" ht="15.75">
@@ -1557,13 +1557,13 @@
       </c>
       <c r="C14" s="11"/>
       <c r="T14" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="15" spans="1:20" ht="18">
       <c r="A15" s="3"/>
       <c r="T15" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="16" spans="1:20" ht="15.75">
@@ -1572,28 +1572,28 @@
       </c>
       <c r="C16" s="10"/>
       <c r="T16" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="17" spans="1:20">
       <c r="T17" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="18" spans="1:20" ht="15">
       <c r="B18" s="7" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C18" s="21" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
     </row>
     <row r="20" spans="1:20" ht="15">
       <c r="B20" s="6" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C20" s="21" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
     </row>
     <row r="21" spans="1:20" ht="15">
@@ -1602,20 +1602,20 @@
     </row>
     <row r="22" spans="1:20" ht="15">
       <c r="B22" s="6" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="C22" s="23"/>
     </row>
     <row r="24" spans="1:20" ht="15">
       <c r="B24" s="6" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="C24" s="9"/>
     </row>
     <row r="26" spans="1:20" ht="18">
       <c r="A26" s="3"/>
       <c r="B26" s="6" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="C26" s="9"/>
     </row>
@@ -1624,18 +1624,18 @@
     </row>
     <row r="28" spans="1:20" ht="15">
       <c r="B28" s="6" t="s">
-        <v>4</v>
+        <v>307</v>
       </c>
       <c r="C28" s="21" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
     </row>
     <row r="30" spans="1:20" ht="15">
       <c r="B30" s="6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
     </row>
     <row r="31" spans="1:20" ht="15">
@@ -1643,7 +1643,7 @@
     </row>
     <row r="32" spans="1:20" ht="15">
       <c r="B32" s="6" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="C32" s="9"/>
     </row>
@@ -1652,10 +1652,10 @@
     </row>
     <row r="34" spans="2:4" ht="15">
       <c r="B34" s="6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="D34" s="1"/>
     </row>
@@ -1665,10 +1665,10 @@
     </row>
     <row r="36" spans="2:4" ht="15">
       <c r="B36" s="6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="D36" s="1"/>
     </row>
@@ -1678,7 +1678,7 @@
     </row>
     <row r="38" spans="2:4" ht="15">
       <c r="B38" s="6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C38" s="9"/>
       <c r="D38" s="1"/>
@@ -1689,19 +1689,19 @@
     </row>
     <row r="40" spans="2:4" ht="15">
       <c r="B40" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="D40" s="1"/>
     </row>
     <row r="42" spans="2:4" ht="15">
       <c r="B42" s="6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="D42" s="1"/>
     </row>
@@ -1762,1107 +1762,1107 @@
     <row r="2" spans="2:2" ht="15.75" thickBot="1"/>
     <row r="3" spans="2:2" ht="16.5" thickBot="1">
       <c r="B3" s="14" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="4" spans="2:2" ht="16.5" thickBot="1">
       <c r="B4" s="15" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="5" spans="2:2" ht="16.5" thickBot="1">
       <c r="B5" s="15" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="6" spans="2:2" ht="16.5" thickBot="1">
       <c r="B6" s="15" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="7" spans="2:2" ht="16.5" thickBot="1">
       <c r="B7" s="15" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="8" spans="2:2" ht="16.5" thickBot="1">
       <c r="B8" s="15" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="9" spans="2:2" ht="16.5" thickBot="1">
       <c r="B9" s="15" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="10" spans="2:2" ht="16.5" thickBot="1">
       <c r="B10" s="15" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="11" spans="2:2" ht="16.5" thickBot="1">
       <c r="B11" s="15" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="12" spans="2:2" ht="16.5" thickBot="1">
       <c r="B12" s="15" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="13" spans="2:2" ht="16.5" thickBot="1">
       <c r="B13" s="15" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="14" spans="2:2" ht="16.5" thickBot="1">
       <c r="B14" s="15" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="15" spans="2:2" ht="16.5" thickBot="1">
       <c r="B15" s="15" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="16" spans="2:2" ht="16.5" thickBot="1">
       <c r="B16" s="15" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="17" spans="2:2" ht="16.5" thickBot="1">
       <c r="B17" s="15" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="18" spans="2:2" ht="16.5" thickBot="1">
       <c r="B18" s="15" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="19" spans="2:2" ht="16.5" thickBot="1">
       <c r="B19" s="15" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="20" spans="2:2" ht="16.5" thickBot="1">
       <c r="B20" s="15" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="21" spans="2:2" ht="16.5" thickBot="1">
       <c r="B21" s="15" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="22" spans="2:2" ht="16.5" thickBot="1">
       <c r="B22" s="15" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="23" spans="2:2" ht="16.5" thickBot="1">
       <c r="B23" s="15" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="24" spans="2:2" ht="16.5" thickBot="1">
       <c r="B24" s="15" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="25" spans="2:2" ht="16.5" thickBot="1">
       <c r="B25" s="15" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="26" spans="2:2" ht="16.5" thickBot="1">
       <c r="B26" s="15" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="27" spans="2:2" ht="16.5" thickBot="1">
       <c r="B27" s="15" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="28" spans="2:2" ht="16.5" thickBot="1">
       <c r="B28" s="15" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="29" spans="2:2" ht="16.5" thickBot="1">
       <c r="B29" s="15" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="30" spans="2:2" ht="16.5" thickBot="1">
       <c r="B30" s="15" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="31" spans="2:2" ht="16.5" thickBot="1">
       <c r="B31" s="15" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="32" spans="2:2" ht="16.5" thickBot="1">
       <c r="B32" s="15" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="33" spans="2:2" ht="16.5" thickBot="1">
       <c r="B33" s="15" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="34" spans="2:2" ht="16.5" thickBot="1">
       <c r="B34" s="15" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="35" spans="2:2" ht="16.5" thickBot="1">
       <c r="B35" s="15" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="36" spans="2:2" ht="16.5" thickBot="1">
       <c r="B36" s="15" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="37" spans="2:2" ht="16.5" thickBot="1">
       <c r="B37" s="15" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="38" spans="2:2" ht="16.5" thickBot="1">
       <c r="B38" s="15" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="39" spans="2:2" ht="16.5" thickBot="1">
       <c r="B39" s="15" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="40" spans="2:2" ht="16.5" thickBot="1">
       <c r="B40" s="15" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="41" spans="2:2" ht="16.5" thickBot="1">
       <c r="B41" s="15" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="42" spans="2:2" ht="16.5" thickBot="1">
       <c r="B42" s="15" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="43" spans="2:2" ht="16.5" thickBot="1">
       <c r="B43" s="15" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="44" spans="2:2" ht="16.5" thickBot="1">
       <c r="B44" s="15" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="45" spans="2:2" ht="16.5" thickBot="1">
       <c r="B45" s="15" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="46" spans="2:2" ht="16.5" thickBot="1">
       <c r="B46" s="15" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="47" spans="2:2" ht="16.5" thickBot="1">
       <c r="B47" s="15" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="48" spans="2:2" ht="16.5" thickBot="1">
       <c r="B48" s="15" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="49" spans="2:2" ht="16.5" thickBot="1">
       <c r="B49" s="15" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="50" spans="2:2" ht="16.5" thickBot="1">
       <c r="B50" s="15" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="51" spans="2:2" ht="16.5" thickBot="1">
       <c r="B51" s="15" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="52" spans="2:2" ht="16.5" thickBot="1">
       <c r="B52" s="15" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="53" spans="2:2" ht="16.5" thickBot="1">
       <c r="B53" s="15" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="54" spans="2:2" ht="16.5" thickBot="1">
       <c r="B54" s="15" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="55" spans="2:2" ht="16.5" thickBot="1">
       <c r="B55" s="15" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="56" spans="2:2" ht="16.5" thickBot="1">
       <c r="B56" s="15" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="57" spans="2:2" ht="16.5" thickBot="1">
       <c r="B57" s="15" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="58" spans="2:2" ht="16.5" thickBot="1">
       <c r="B58" s="15" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="59" spans="2:2" ht="16.5" thickBot="1">
       <c r="B59" s="15" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="60" spans="2:2" ht="16.5" thickBot="1">
       <c r="B60" s="15" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="61" spans="2:2" ht="16.5" thickBot="1">
       <c r="B61" s="15" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="62" spans="2:2" ht="16.5" thickBot="1">
       <c r="B62" s="15" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="63" spans="2:2" ht="16.5" thickBot="1">
       <c r="B63" s="15" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="64" spans="2:2" ht="16.5" thickBot="1">
       <c r="B64" s="15" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="65" spans="2:2" ht="16.5" thickBot="1">
       <c r="B65" s="15" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="66" spans="2:2" ht="16.5" thickBot="1">
       <c r="B66" s="15" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="67" spans="2:2" ht="16.5" thickBot="1">
       <c r="B67" s="15" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="68" spans="2:2" ht="16.5" thickBot="1">
       <c r="B68" s="15" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="69" spans="2:2" ht="16.5" thickBot="1">
       <c r="B69" s="15" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="70" spans="2:2" ht="16.5" thickBot="1">
       <c r="B70" s="15" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="71" spans="2:2" ht="16.5" thickBot="1">
       <c r="B71" s="15" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="72" spans="2:2" ht="16.5" thickBot="1">
       <c r="B72" s="15" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="73" spans="2:2" ht="16.5" thickBot="1">
       <c r="B73" s="15" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="74" spans="2:2" ht="16.5" thickBot="1">
       <c r="B74" s="15" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="75" spans="2:2" ht="16.5" thickBot="1">
       <c r="B75" s="15" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="76" spans="2:2" ht="16.5" thickBot="1">
       <c r="B76" s="15" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="77" spans="2:2" ht="16.5" thickBot="1">
       <c r="B77" s="15" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="78" spans="2:2" ht="16.5" thickBot="1">
       <c r="B78" s="15" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="79" spans="2:2" ht="16.5" thickBot="1">
       <c r="B79" s="15" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="80" spans="2:2" ht="16.5" thickBot="1">
       <c r="B80" s="15" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="81" spans="2:2" ht="16.5" thickBot="1">
       <c r="B81" s="15" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="82" spans="2:2" ht="16.5" thickBot="1">
       <c r="B82" s="15" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="83" spans="2:2" ht="16.5" thickBot="1">
       <c r="B83" s="15" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="84" spans="2:2" ht="16.5" thickBot="1">
       <c r="B84" s="15" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="85" spans="2:2" ht="16.5" thickBot="1">
       <c r="B85" s="15" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="86" spans="2:2" ht="16.5" thickBot="1">
       <c r="B86" s="15" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="87" spans="2:2" ht="16.5" thickBot="1">
       <c r="B87" s="15" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="88" spans="2:2" ht="16.5" thickBot="1">
       <c r="B88" s="15" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="89" spans="2:2" ht="16.5" thickBot="1">
       <c r="B89" s="15" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="90" spans="2:2" ht="16.5" thickBot="1">
       <c r="B90" s="15" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="91" spans="2:2" ht="16.5" thickBot="1">
       <c r="B91" s="15" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="92" spans="2:2" ht="16.5" thickBot="1">
       <c r="B92" s="15" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="93" spans="2:2" ht="16.5" thickBot="1">
       <c r="B93" s="15" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="94" spans="2:2" ht="16.5" thickBot="1">
       <c r="B94" s="15" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="95" spans="2:2" ht="16.5" thickBot="1">
       <c r="B95" s="15" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="96" spans="2:2" ht="16.5" thickBot="1">
       <c r="B96" s="15" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="97" spans="2:2" ht="16.5" thickBot="1">
       <c r="B97" s="15" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="98" spans="2:2" ht="16.5" thickBot="1">
       <c r="B98" s="15" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="99" spans="2:2" ht="16.5" thickBot="1">
       <c r="B99" s="15" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="100" spans="2:2" ht="16.5" thickBot="1">
       <c r="B100" s="15" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="101" spans="2:2" ht="16.5" thickBot="1">
       <c r="B101" s="15" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="102" spans="2:2" ht="16.5" thickBot="1">
       <c r="B102" s="15" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="103" spans="2:2" ht="16.5" thickBot="1">
       <c r="B103" s="15" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="104" spans="2:2" ht="16.5" thickBot="1">
       <c r="B104" s="15" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="105" spans="2:2" ht="16.5" thickBot="1">
       <c r="B105" s="15" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="106" spans="2:2" ht="16.5" thickBot="1">
       <c r="B106" s="15" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="107" spans="2:2" ht="16.5" thickBot="1">
       <c r="B107" s="15" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="108" spans="2:2" ht="16.5" thickBot="1">
       <c r="B108" s="15" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="109" spans="2:2" ht="16.5" thickBot="1">
       <c r="B109" s="15" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="110" spans="2:2" ht="16.5" thickBot="1">
       <c r="B110" s="15" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="111" spans="2:2" ht="16.5" thickBot="1">
       <c r="B111" s="15" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="112" spans="2:2" ht="16.5" thickBot="1">
       <c r="B112" s="15" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="113" spans="2:2" ht="16.5" thickBot="1">
       <c r="B113" s="15" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="114" spans="2:2" ht="16.5" thickBot="1">
       <c r="B114" s="15" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="115" spans="2:2" ht="16.5" thickBot="1">
       <c r="B115" s="15" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="116" spans="2:2" ht="16.5" thickBot="1">
       <c r="B116" s="15" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="117" spans="2:2" ht="16.5" thickBot="1">
       <c r="B117" s="15" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="118" spans="2:2" ht="16.5" thickBot="1">
       <c r="B118" s="15" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="119" spans="2:2" ht="16.5" thickBot="1">
       <c r="B119" s="15" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="120" spans="2:2" ht="16.5" thickBot="1">
       <c r="B120" s="15" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="121" spans="2:2" ht="16.5" thickBot="1">
       <c r="B121" s="15" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="122" spans="2:2" ht="16.5" thickBot="1">
       <c r="B122" s="15" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="123" spans="2:2" ht="16.5" thickBot="1">
       <c r="B123" s="15" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="124" spans="2:2" ht="16.5" thickBot="1">
       <c r="B124" s="15" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="125" spans="2:2" ht="16.5" thickBot="1">
       <c r="B125" s="15" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="126" spans="2:2" ht="16.5" thickBot="1">
       <c r="B126" s="15" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="127" spans="2:2" ht="16.5" thickBot="1">
       <c r="B127" s="15" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="128" spans="2:2" ht="16.5" thickBot="1">
       <c r="B128" s="15" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="129" spans="2:2" ht="16.5" thickBot="1">
       <c r="B129" s="15" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="130" spans="2:2" ht="16.5" thickBot="1">
       <c r="B130" s="15" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="131" spans="2:2" ht="16.5" thickBot="1">
       <c r="B131" s="15" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="132" spans="2:2" ht="16.5" thickBot="1">
       <c r="B132" s="15" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="133" spans="2:2" ht="16.5" thickBot="1">
       <c r="B133" s="15" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="134" spans="2:2" ht="16.5" thickBot="1">
       <c r="B134" s="15" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="135" spans="2:2" ht="16.5" thickBot="1">
       <c r="B135" s="15" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="136" spans="2:2" ht="16.5" thickBot="1">
       <c r="B136" s="15" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="137" spans="2:2" ht="16.5" thickBot="1">
       <c r="B137" s="15" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="138" spans="2:2" ht="16.5" thickBot="1">
       <c r="B138" s="15" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="139" spans="2:2" ht="16.5" thickBot="1">
       <c r="B139" s="15" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="140" spans="2:2" ht="16.5" thickBot="1">
       <c r="B140" s="15" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="141" spans="2:2" ht="16.5" thickBot="1">
       <c r="B141" s="15" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="142" spans="2:2" ht="16.5" thickBot="1">
       <c r="B142" s="15" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="143" spans="2:2" ht="16.5" thickBot="1">
       <c r="B143" s="15" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="144" spans="2:2" ht="16.5" thickBot="1">
       <c r="B144" s="15" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="145" spans="2:2" ht="16.5" thickBot="1">
       <c r="B145" s="15" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="146" spans="2:2" ht="16.5" thickBot="1">
       <c r="B146" s="15" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="147" spans="2:2" ht="16.5" thickBot="1">
       <c r="B147" s="15" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="148" spans="2:2" ht="16.5" thickBot="1">
       <c r="B148" s="15" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="149" spans="2:2" ht="16.5" thickBot="1">
       <c r="B149" s="15" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="150" spans="2:2" ht="16.5" thickBot="1">
       <c r="B150" s="15" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="151" spans="2:2" ht="16.5" thickBot="1">
       <c r="B151" s="15" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="152" spans="2:2" ht="16.5" thickBot="1">
       <c r="B152" s="15" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="153" spans="2:2" ht="16.5" thickBot="1">
       <c r="B153" s="15" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="154" spans="2:2" ht="16.5" thickBot="1">
       <c r="B154" s="15" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="155" spans="2:2" ht="16.5" thickBot="1">
       <c r="B155" s="15" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="156" spans="2:2" ht="16.5" thickBot="1">
       <c r="B156" s="15" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="157" spans="2:2" ht="16.5" thickBot="1">
       <c r="B157" s="15" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="158" spans="2:2" ht="16.5" thickBot="1">
       <c r="B158" s="15" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="159" spans="2:2" ht="16.5" thickBot="1">
       <c r="B159" s="15" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="160" spans="2:2" ht="16.5" thickBot="1">
       <c r="B160" s="15" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="161" spans="2:2" ht="16.5" thickBot="1">
       <c r="B161" s="15" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="162" spans="2:2" ht="16.5" thickBot="1">
       <c r="B162" s="15" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="163" spans="2:2" ht="16.5" thickBot="1">
       <c r="B163" s="15" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="164" spans="2:2" ht="16.5" thickBot="1">
       <c r="B164" s="15" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="165" spans="2:2" ht="16.5" thickBot="1">
       <c r="B165" s="15" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="166" spans="2:2" ht="16.5" thickBot="1">
       <c r="B166" s="15" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="167" spans="2:2" ht="16.5" thickBot="1">
       <c r="B167" s="15" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="168" spans="2:2" ht="16.5" thickBot="1">
       <c r="B168" s="15" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="169" spans="2:2" ht="16.5" thickBot="1">
       <c r="B169" s="15" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="170" spans="2:2" ht="16.5" thickBot="1">
       <c r="B170" s="15" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="171" spans="2:2" ht="16.5" thickBot="1">
       <c r="B171" s="15" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="172" spans="2:2" ht="16.5" thickBot="1">
       <c r="B172" s="15" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="173" spans="2:2" ht="16.5" thickBot="1">
       <c r="B173" s="15" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="174" spans="2:2" ht="16.5" thickBot="1">
       <c r="B174" s="15" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="175" spans="2:2" ht="16.5" thickBot="1">
       <c r="B175" s="15" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="176" spans="2:2" ht="16.5" thickBot="1">
       <c r="B176" s="15" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="177" spans="2:2" ht="16.5" thickBot="1">
       <c r="B177" s="15" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="178" spans="2:2" ht="16.5" thickBot="1">
       <c r="B178" s="15" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="179" spans="2:2" ht="16.5" thickBot="1">
       <c r="B179" s="15" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="180" spans="2:2" ht="16.5" thickBot="1">
       <c r="B180" s="15" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="181" spans="2:2" ht="16.5" thickBot="1">
       <c r="B181" s="15" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="182" spans="2:2" ht="16.5" thickBot="1">
       <c r="B182" s="15" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="183" spans="2:2" ht="16.5" thickBot="1">
       <c r="B183" s="15" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="184" spans="2:2" ht="16.5" thickBot="1">
       <c r="B184" s="15" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="185" spans="2:2" ht="16.5" thickBot="1">
       <c r="B185" s="15" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="186" spans="2:2" ht="16.5" thickBot="1">
       <c r="B186" s="15" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="187" spans="2:2" ht="16.5" thickBot="1">
       <c r="B187" s="15" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="188" spans="2:2" ht="16.5" thickBot="1">
       <c r="B188" s="15" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="189" spans="2:2" ht="16.5" thickBot="1">
       <c r="B189" s="15" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="190" spans="2:2" ht="16.5" thickBot="1">
       <c r="B190" s="15" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="191" spans="2:2" ht="16.5" thickBot="1">
       <c r="B191" s="15" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="192" spans="2:2" ht="16.5" thickBot="1">
       <c r="B192" s="15" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="193" spans="2:2" ht="16.5" thickBot="1">
       <c r="B193" s="15" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="194" spans="2:2" ht="16.5" thickBot="1">
       <c r="B194" s="15" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="195" spans="2:2" ht="16.5" thickBot="1">
       <c r="B195" s="15" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="196" spans="2:2" ht="16.5" thickBot="1">
       <c r="B196" s="15" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="197" spans="2:2" ht="16.5" thickBot="1">
       <c r="B197" s="15" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="198" spans="2:2" ht="16.5" thickBot="1">
       <c r="B198" s="15" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="199" spans="2:2" ht="16.5" thickBot="1">
       <c r="B199" s="15" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="200" spans="2:2" ht="16.5" thickBot="1">
       <c r="B200" s="15" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="201" spans="2:2" ht="16.5" thickBot="1">
       <c r="B201" s="15" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="202" spans="2:2" ht="16.5" thickBot="1">
       <c r="B202" s="15" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="203" spans="2:2" ht="16.5" thickBot="1">
       <c r="B203" s="15" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="204" spans="2:2" ht="16.5" thickBot="1">
       <c r="B204" s="15" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="205" spans="2:2" ht="16.5" thickBot="1">
       <c r="B205" s="15" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="206" spans="2:2" ht="16.5" thickBot="1">
       <c r="B206" s="15" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="207" spans="2:2" ht="16.5" thickBot="1">
       <c r="B207" s="15" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="208" spans="2:2" ht="16.5" thickBot="1">
       <c r="B208" s="15" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="209" spans="2:2" ht="16.5" thickBot="1">
       <c r="B209" s="15" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="210" spans="2:2" ht="16.5" thickBot="1">
       <c r="B210" s="15" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="211" spans="2:2" ht="16.5" thickBot="1">
       <c r="B211" s="15" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="212" spans="2:2" ht="16.5" thickBot="1">
       <c r="B212" s="15" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="213" spans="2:2" ht="16.5" thickBot="1">
       <c r="B213" s="15" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="214" spans="2:2" ht="16.5" thickBot="1">
       <c r="B214" s="15" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="215" spans="2:2" ht="16.5" thickBot="1">
       <c r="B215" s="15" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="216" spans="2:2" ht="16.5" thickBot="1">
       <c r="B216" s="15" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="217" spans="2:2" ht="16.5" thickBot="1">
       <c r="B217" s="15" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="218" spans="2:2" ht="16.5" thickBot="1">
       <c r="B218" s="15" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="219" spans="2:2" ht="16.5" thickBot="1">
       <c r="B219" s="15" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="220" spans="2:2" ht="16.5" thickBot="1">
       <c r="B220" s="15" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="221" spans="2:2" ht="16.5" thickBot="1">
       <c r="B221" s="15" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="222" spans="2:2" ht="16.5" thickBot="1">
       <c r="B222" s="15" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="223" spans="2:2" ht="16.5" thickBot="1">
       <c r="B223" s="15" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
   </sheetData>
@@ -2889,220 +2889,220 @@
   <sheetData>
     <row r="2" spans="2:6">
       <c r="B2" s="16" t="s">
+        <v>266</v>
+      </c>
+      <c r="C2" s="18" t="s">
         <v>267</v>
       </c>
-      <c r="C2" s="18" t="s">
+      <c r="D2" s="18" t="s">
+        <v>269</v>
+      </c>
+      <c r="E2" s="18" t="s">
         <v>268</v>
       </c>
-      <c r="D2" s="18" t="s">
-        <v>270</v>
-      </c>
-      <c r="E2" s="18" t="s">
-        <v>269</v>
-      </c>
       <c r="F2" s="18" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
     </row>
     <row r="3" spans="2:6">
       <c r="B3" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="C3" t="s">
+        <v>270</v>
+      </c>
+      <c r="D3" t="s">
         <v>271</v>
       </c>
-      <c r="D3" t="s">
-        <v>272</v>
-      </c>
       <c r="E3" s="17" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="F3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="4" spans="2:6">
       <c r="B4" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="C4" t="s">
+        <v>272</v>
+      </c>
+      <c r="D4" t="s">
         <v>273</v>
       </c>
-      <c r="D4" t="s">
-        <v>274</v>
-      </c>
       <c r="E4" s="17" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="F4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="5" spans="2:6">
       <c r="B5" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="C5" t="s">
+        <v>274</v>
+      </c>
+      <c r="D5" t="s">
         <v>275</v>
       </c>
-      <c r="D5" t="s">
-        <v>276</v>
-      </c>
       <c r="E5" s="17" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="F5" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="6" spans="2:6">
       <c r="B6" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="C6" t="s">
+        <v>276</v>
+      </c>
+      <c r="D6" t="s">
         <v>277</v>
       </c>
-      <c r="D6" t="s">
-        <v>278</v>
-      </c>
       <c r="E6" s="17" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="F6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="7" spans="2:6">
       <c r="B7" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="C7" t="s">
+        <v>278</v>
+      </c>
+      <c r="D7" t="s">
         <v>279</v>
       </c>
-      <c r="D7" t="s">
-        <v>280</v>
-      </c>
       <c r="F7" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
     </row>
     <row r="8" spans="2:6">
       <c r="B8" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="C8" t="s">
+        <v>280</v>
+      </c>
+      <c r="D8" t="s">
         <v>281</v>
       </c>
-      <c r="D8" t="s">
-        <v>282</v>
-      </c>
       <c r="F8" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
     </row>
     <row r="9" spans="2:6">
       <c r="B9" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="D9" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="F9" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
     </row>
     <row r="10" spans="2:6">
       <c r="B10" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="D10" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="F10" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="11" spans="2:6">
       <c r="B11" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="F11" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
     </row>
     <row r="12" spans="2:6">
       <c r="B12" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="F12" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
     </row>
     <row r="13" spans="2:6">
       <c r="B13" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="F13" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
     </row>
     <row r="14" spans="2:6">
       <c r="B14" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="F14" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
     </row>
     <row r="15" spans="2:6">
       <c r="B15" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="F15" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
     </row>
     <row r="16" spans="2:6">
       <c r="B16" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="F16" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="17" spans="2:2">
       <c r="B17" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="18" spans="2:2">
       <c r="B18" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="19" spans="2:2">
       <c r="B19" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
     <row r="20" spans="2:2">
       <c r="B20" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="21" spans="2:2">
       <c r="B21" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="22" spans="2:2">
       <c r="B22" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="23" spans="2:2">
       <c r="B23" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
   </sheetData>

</xml_diff>